<commit_message>
fix: update the script to plot figures
</commit_message>
<xml_diff>
--- a/data/Yeast_fermentation_data.xlsx
+++ b/data/Yeast_fermentation_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/Google Drive/R application and code/protein 3D structure QC and QA/graph_evolution_result/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/Documents/GitHub/R_code_for_graph_in_evolution/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2BF88B-DD18-5C4C-84FD-255FA3C0CB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A225B8-CDA9-5641-A21A-D60C145E435E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{288FD51C-80D7-8D4E-AE76-CB2F7DCD0299}"/>
   </bookViews>
@@ -7632,10 +7632,10 @@
   <dimension ref="A1:M162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B74" sqref="B74:B81"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>